<commit_message>
archivos de UMBooK importados desde Drive
</commit_message>
<xml_diff>
--- a/Clases de los casos de Uso.xlsx
+++ b/Clases de los casos de Uso.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Iniciar Sesion</t>
   </si>
@@ -320,16 +320,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -341,6 +331,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -660,15 +660,15 @@
       <c r="J2" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="17" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="17" t="s">
         <v>2</v>
       </c>
       <c r="G3" s="4"/>
@@ -676,7 +676,7 @@
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="18" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -693,7 +693,7 @@
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="5"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
@@ -702,12 +702,10 @@
         <v>7</v>
       </c>
       <c r="G5" s="4"/>
-      <c r="I5" s="1" t="s">
-        <v>29</v>
-      </c>
+      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="7"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="5"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
@@ -718,7 +716,7 @@
       <c r="G6" s="4"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="5"/>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
@@ -729,7 +727,7 @@
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="7"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
@@ -741,7 +739,7 @@
       <c r="J8" s="1"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="7"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="5"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
@@ -754,7 +752,7 @@
       <c r="J9" s="1"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -773,7 +771,7 @@
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
@@ -790,7 +788,7 @@
       <c r="J11" s="1"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="7"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="5"/>
       <c r="C12" s="4"/>
       <c r="D12" s="3" t="s">
@@ -806,7 +804,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="5"/>
       <c r="C13" s="4"/>
       <c r="D13" s="3" t="s">
@@ -819,7 +817,7 @@
       <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="8"/>
+      <c r="A14" s="20"/>
       <c r="B14" s="5"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
@@ -830,7 +828,7 @@
       <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="18" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -847,7 +845,7 @@
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="5"/>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
@@ -858,7 +856,7 @@
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
+      <c r="A17" s="19"/>
       <c r="B17" s="5"/>
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
@@ -867,7 +865,7 @@
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="8"/>
+      <c r="A18" s="20"/>
       <c r="B18" s="5"/>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
@@ -876,133 +874,133 @@
       <c r="G18" s="4"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="14"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="17"/>
+      <c r="A23" s="9"/>
+      <c r="B23" s="10"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="10"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="11"/>
     </row>
     <row r="24" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="20"/>
+      <c r="A24" s="12"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="14"/>
     </row>
     <row r="26" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="14"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="17"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="11"/>
     </row>
     <row r="29" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
+      <c r="A29" s="9"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="11"/>
     </row>
     <row r="30" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="18"/>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="20"/>
+      <c r="A30" s="12"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="32" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
       <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="14"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="8"/>
     </row>
     <row r="34" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="15"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="17"/>
+      <c r="A34" s="9"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="11"/>
     </row>
     <row r="35" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="18"/>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="20"/>
+      <c r="A35" s="12"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+      <c r="G35" s="14"/>
     </row>
     <row r="41" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2"/>
@@ -1219,28 +1217,24 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="A22:G24"/>
-    <mergeCell ref="A21:G21"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A33:G35"/>
-    <mergeCell ref="A32:G32"/>
-    <mergeCell ref="A27:G30"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D8:E8"/>
     <mergeCell ref="A4:A9"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="D6:E6"/>
@@ -1257,25 +1251,29 @@
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:C16"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="A33:G35"/>
+    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A27:G30"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="A22:G24"/>
+    <mergeCell ref="A21:G21"/>
+    <mergeCell ref="A26:G26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
nuevos clases de casos de uso
</commit_message>
<xml_diff>
--- a/Clases de los casos de Uso.xlsx
+++ b/Clases de los casos de Uso.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
     <t>Iniciar Sesion</t>
   </si>
@@ -51,7 +51,7 @@
     <t>Subir foto</t>
   </si>
   <si>
-    <t>Crear album                     </t>
+    <t>Crear album</t>
   </si>
   <si>
     <t>Clases de Control</t>
@@ -99,7 +99,7 @@
     <t>El usuario completa el formulario de registro y luego envia la solicitud de registro. El sistema analiza el formulario ingresado, verificando: que no existan campos en blanco, que la contraseña cumpla con los requisitos, que el e-mail esté bien ingrado y no tenga otra cuenta registrada, se hayan aceptado los terminos y condiciones. Para ello, compara los datos ingreados en la base de datos Usuarios. Si existe mal ingresado, el sistema devuelve un mensaje de aviso indicando donde se encuentra el error.</t>
   </si>
   <si>
-    <t>En Gestionar Muro, el usuario accede a las opciones que le permiten editar su muro, comentarios, amigos, fotos, albumes. Cuando el usuario ingresa un comentario verifica los permisos concedidos a los otros usuarios. Al subir una foto, verifica si la extencion del archivo es validad para el sistema. Cuando se busca un amigo, el sistema busca coincidencias del nombre ingresado con los nombres de la base de datos Usuarios. </t>
+    <t>En Gestionar Muro, el usuario accede a las opciones que le permiten editar su muro, comentarios, amigos, fotos, albumes. Cuando el usuario ingresa un comentario verifica los permisos concedidos a los otros usuarios. Al subir una foto, verifica si la extencion del archivo es validad para el sistema. Cuando se busca un amigo, el sistema busca coincidencias del nombre ingresado con los nombres de la base de datos Usuarios.</t>
   </si>
   <si>
     <t>Buscar Amigos</t>
@@ -111,12 +111,57 @@
     <t>Crear Grupo de Amigos</t>
   </si>
   <si>
+    <t>Definir Privacidad de Grupo</t>
+  </si>
+  <si>
+    <t>Adminsitrar Cumpleaños</t>
+  </si>
+  <si>
+    <t>Modificar Comentario</t>
+  </si>
+  <si>
+    <t>Gestionar solicitud amistad</t>
+  </si>
+  <si>
+    <t>Crear Album</t>
+  </si>
+  <si>
     <t>Interfaz</t>
   </si>
   <si>
     <t>Enviar Solicitud de Amistad</t>
   </si>
   <si>
+    <t>Elejir Privacidad</t>
+  </si>
+  <si>
+    <t>Ingresar Nº Antisipacion de Cumpleaños</t>
+  </si>
+  <si>
+    <t>Ingresar nuevo comentario</t>
+  </si>
+  <si>
+    <t>Ver Solicitud/es de amistad</t>
+  </si>
+  <si>
+    <t>Ingresare nombre </t>
+  </si>
+  <si>
+    <t>Opcion: agregar comentario</t>
+  </si>
+  <si>
+    <t>Opcion: Ingresar lugar donde se tomaron las fotos</t>
+  </si>
+  <si>
+    <t>Agregar fotos</t>
+  </si>
+  <si>
+    <t>Opcion: Agregar comentarios sobre una foto</t>
+  </si>
+  <si>
+    <t>Publicar</t>
+  </si>
+  <si>
     <t>Control</t>
   </si>
   <si>
@@ -126,16 +171,49 @@
     <t>Mostrar que la solicitud fue enviada</t>
   </si>
   <si>
-    <t>Mostrar resultados</t>
+    <t>Verificar Existencia de Nombre</t>
+  </si>
+  <si>
+    <t>Aplicar Privacidad</t>
+  </si>
+  <si>
+    <t>Verificar Numero Ingresado</t>
+  </si>
+  <si>
+    <t>Agregar comentario nuevo</t>
+  </si>
+  <si>
+    <t>Verificar Respuesta elegida</t>
+  </si>
+  <si>
+    <t>verificar formato de fotos</t>
   </si>
   <si>
     <t>Notificar al usuario invitado</t>
   </si>
   <si>
+    <t>enviar a amigo notificacion de respuesta</t>
+  </si>
+  <si>
+    <t>verificar tamaño de fotos</t>
+  </si>
+  <si>
     <t>Entidad</t>
   </si>
   <si>
-    <t>Especificación</t>
+    <t>Grupos</t>
+  </si>
+  <si>
+    <t>Amigos</t>
+  </si>
+  <si>
+    <t>muro</t>
+  </si>
+  <si>
+    <t>Notificaciones</t>
+  </si>
+  <si>
+    <t>Albums</t>
   </si>
   <si>
     <t>Buscar amigos</t>
@@ -151,6 +229,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">umBook</t>
     </r>
@@ -160,6 +239,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> el nombre del usuario. Se compara la cadena de texto ingresada con los nombres de usuarios almacenados en la tabla de </t>
     </r>
@@ -170,6 +250,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Usuarios</t>
     </r>
@@ -179,6 +260,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> del sistema. Y  muestra las coincidencias. Una vez hecho esto, verificara si forma parte de los amigos, si forma parte de los amigos no incluira la opcion de enviar solicitud, y viceversa.</t>
     </r>
@@ -231,10 +313,12 @@
       <charset val="1"/>
     </font>
     <font>
+      <u val="single"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -242,6 +326,7 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -276,7 +361,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -314,6 +399,13 @@
     </border>
     <border diagonalUp="false" diagonalDown="false">
       <left style="hair"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
       <right style="hair"/>
       <top/>
       <bottom/>
@@ -352,7 +444,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -405,10 +497,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -417,7 +517,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="justify" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -501,7 +605,7 @@
   <dimension ref="A1:Z1004"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="1" sqref="C:C I5"/>
+      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1146,15 +1250,21 @@
   <dimension ref="A3:L27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.6275510204082"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="30.1938775510204"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="26.4387755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="33.9438775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.9642857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="34.0816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="41.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1167,61 +1277,85 @@
       <c r="D3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="E3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="J3" s="10"/>
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
+      <c r="E4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="J4" s="12"/>
       <c r="K4" s="12"/>
       <c r="L4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="12" t="s">
+        <v>43</v>
+      </c>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="12" t="s">
+        <v>44</v>
+      </c>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
@@ -1229,93 +1363,107 @@
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11"/>
       <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="12" t="s">
+        <v>45</v>
+      </c>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="12" t="s">
+        <v>46</v>
+      </c>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="11"/>
-      <c r="B9" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
+      <c r="A10" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>56</v>
+      </c>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="11"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12" t="s">
+        <v>57</v>
+      </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
+      <c r="H11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>59</v>
+      </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>23</v>
-      </c>
+      <c r="A12" s="11"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -1328,8 +1476,8 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="B13" s="18"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
@@ -1341,15 +1489,33 @@
       <c r="L13" s="12"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="A14" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
@@ -1368,144 +1534,161 @@
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
     </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="11"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+    </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>39</v>
-      </c>
+      <c r="A17" s="11"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="16"/>
+        <v>66</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="11"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="11"/>
-      <c r="B20" s="16"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="16"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="11"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="16"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
+      <c r="B22" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="11"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="16"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="11"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="11"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="16"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="11"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="16"/>
-      <c r="J26" s="16"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="11"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="16"/>
-      <c r="J27" s="16"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="B18:J21"/>
     <mergeCell ref="A22:A27"/>
@@ -1515,8 +1698,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Página &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>